<commit_message>
did almost all the controls merge
</commit_message>
<xml_diff>
--- a/data/reg_dif_med_results/difmedias_entre_anos_2019x2011.xlsx
+++ b/data/reg_dif_med_results/difmedias_entre_anos_2019x2011.xlsx
@@ -417,16 +417,16 @@
     <t>0.029</t>
   </si>
   <si>
-    <t>16746</t>
-  </si>
-  <si>
-    <t>17614</t>
+    <t>16748</t>
+  </si>
+  <si>
+    <t>17616</t>
   </si>
   <si>
     <t>13516</t>
   </si>
   <si>
-    <t>16034</t>
+    <t>16036</t>
   </si>
   <si>
     <t xml:space="preserve"> (2) </t>
@@ -441,7 +441,7 @@
     <t>(0.008)</t>
   </si>
   <si>
-    <t>39.314</t>
+    <t>39.307</t>
   </si>
   <si>
     <t>(0.574)</t>
@@ -462,13 +462,13 @@
     <t>(0.011)</t>
   </si>
   <si>
-    <t>4.072</t>
+    <t>4.068</t>
   </si>
   <si>
     <t>(0.059)</t>
   </si>
   <si>
-    <t>6.970</t>
+    <t>6.962</t>
   </si>
   <si>
     <t>(0.076)</t>
@@ -480,7 +480,7 @@
     <t>0.148</t>
   </si>
   <si>
-    <t>0.197</t>
+    <t>0.198</t>
   </si>
   <si>
     <t>0.025</t>
@@ -492,6 +492,9 @@
     <t>0.069</t>
   </si>
   <si>
+    <t>0.200</t>
+  </si>
+  <si>
     <t>0.111</t>
   </si>
   <si>
@@ -516,7 +519,7 @@
     <t>0.160</t>
   </si>
   <si>
-    <t>0.432</t>
+    <t>0.433</t>
   </si>
   <si>
     <t>0.039</t>
@@ -528,9 +531,6 @@
     <t>0.055</t>
   </si>
   <si>
-    <t>0.030</t>
-  </si>
-  <si>
     <t>0.084</t>
   </si>
   <si>
@@ -552,19 +552,19 @@
     <t>0.053</t>
   </si>
   <si>
-    <t>0.328</t>
-  </si>
-  <si>
-    <t>28129</t>
-  </si>
-  <si>
-    <t>28997</t>
+    <t>0.329</t>
+  </si>
+  <si>
+    <t>28131</t>
+  </si>
+  <si>
+    <t>28999</t>
   </si>
   <si>
     <t>24899</t>
   </si>
   <si>
-    <t>27417</t>
+    <t>27419</t>
   </si>
   <si>
     <t>(2)-(1)</t>
@@ -579,22 +579,22 @@
     <t>-0.031**</t>
   </si>
   <si>
-    <t>1.483**</t>
+    <t>1.476**</t>
   </si>
   <si>
     <t>-0.002**</t>
   </si>
   <si>
-    <t>-0.383***</t>
-  </si>
-  <si>
-    <t>-0.316***</t>
-  </si>
-  <si>
-    <t>-1.177***</t>
-  </si>
-  <si>
-    <t>1.541***</t>
+    <t>-0.382***</t>
+  </si>
+  <si>
+    <t>-0.317***</t>
+  </si>
+  <si>
+    <t>-1.181***</t>
+  </si>
+  <si>
+    <t>1.533***</t>
   </si>
   <si>
     <t>-0.005**</t>
@@ -612,10 +612,13 @@
     <t>0.028***</t>
   </si>
   <si>
+    <t>-0.001</t>
+  </si>
+  <si>
     <t>-0.000</t>
   </si>
   <si>
-    <t>0.034***</t>
+    <t>0.035***</t>
   </si>
   <si>
     <t>-0.262***</t>
@@ -636,7 +639,7 @@
     <t>0.053***</t>
   </si>
   <si>
-    <t>0.096***</t>
+    <t>0.097***</t>
   </si>
   <si>
     <t>-0.003**</t>
@@ -648,10 +651,10 @@
     <t>0.010***</t>
   </si>
   <si>
-    <t>-0.095***</t>
-  </si>
-  <si>
-    <t>-0.001</t>
+    <t>-0.094***</t>
+  </si>
+  <si>
+    <t>-0.002</t>
   </si>
   <si>
     <t>0.008***</t>
@@ -660,7 +663,7 @@
     <t>0.004***</t>
   </si>
   <si>
-    <t>0.017***</t>
+    <t>0.018***</t>
   </si>
   <si>
     <t>-0.003***</t>
@@ -672,15 +675,12 @@
     <t>0.009***</t>
   </si>
   <si>
-    <t>0.007***</t>
+    <t>0.006***</t>
   </si>
   <si>
     <t>0.070***</t>
   </si>
   <si>
-    <t>-0.002</t>
-  </si>
-  <si>
     <t>0.001*</t>
   </si>
   <si>
@@ -690,6 +690,9 @@
     <t>0.063***</t>
   </si>
   <si>
+    <t>-0.006**</t>
+  </si>
+  <si>
     <t>-0.004***</t>
   </si>
   <si>
@@ -703,9 +706,6 @@
   </si>
   <si>
     <t>-0.126***</t>
-  </si>
-  <si>
-    <t>0.006***</t>
   </si>
   <si>
     <t>-0.006</t>
@@ -1463,7 +1463,7 @@
         <v>181</v>
       </c>
       <c r="G30" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="31">
@@ -1595,7 +1595,7 @@
         <v>135</v>
       </c>
       <c r="E36" t="s">
-        <v>100</v>
+        <v>159</v>
       </c>
       <c r="F36" t="s">
         <v>181</v>
@@ -1647,7 +1647,7 @@
         <v>181</v>
       </c>
       <c r="G38" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="39">
@@ -1687,13 +1687,13 @@
         <v>135</v>
       </c>
       <c r="E40" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F40" t="s">
         <v>181</v>
       </c>
       <c r="G40" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="41">
@@ -1779,13 +1779,13 @@
         <v>135</v>
       </c>
       <c r="E44" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F44" t="s">
         <v>181</v>
       </c>
       <c r="G44" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="45">
@@ -1825,13 +1825,13 @@
         <v>135</v>
       </c>
       <c r="E46" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F46" t="s">
         <v>181</v>
       </c>
       <c r="G46" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="47">
@@ -1871,13 +1871,13 @@
         <v>135</v>
       </c>
       <c r="E48" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F48" t="s">
         <v>181</v>
       </c>
       <c r="G48" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="49">
@@ -1917,13 +1917,13 @@
         <v>135</v>
       </c>
       <c r="E50" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F50" t="s">
         <v>181</v>
       </c>
       <c r="G50" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="51">
@@ -1963,7 +1963,7 @@
         <v>135</v>
       </c>
       <c r="E52" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F52" t="s">
         <v>181</v>
@@ -2009,13 +2009,13 @@
         <v>135</v>
       </c>
       <c r="E54" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F54" t="s">
         <v>181</v>
       </c>
       <c r="G54" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="55">
@@ -2055,13 +2055,13 @@
         <v>135</v>
       </c>
       <c r="E56" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F56" t="s">
         <v>181</v>
       </c>
       <c r="G56" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="57">
@@ -2101,13 +2101,13 @@
         <v>135</v>
       </c>
       <c r="E58" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F58" t="s">
         <v>181</v>
       </c>
       <c r="G58" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="59">
@@ -2153,7 +2153,7 @@
         <v>181</v>
       </c>
       <c r="G60" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="61">
@@ -2239,13 +2239,13 @@
         <v>135</v>
       </c>
       <c r="E64" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F64" t="s">
         <v>181</v>
       </c>
       <c r="G64" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="65">
@@ -2291,7 +2291,7 @@
         <v>181</v>
       </c>
       <c r="G66" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="67">
@@ -2331,13 +2331,13 @@
         <v>135</v>
       </c>
       <c r="E68" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F68" t="s">
         <v>181</v>
       </c>
       <c r="G68" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="69">
@@ -2377,13 +2377,13 @@
         <v>135</v>
       </c>
       <c r="E70" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F70" t="s">
         <v>181</v>
       </c>
       <c r="G70" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="71">
@@ -2429,7 +2429,7 @@
         <v>181</v>
       </c>
       <c r="G72" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="73">
@@ -2475,7 +2475,7 @@
         <v>181</v>
       </c>
       <c r="G74" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="75">
@@ -2515,13 +2515,13 @@
         <v>135</v>
       </c>
       <c r="E76" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="F76" t="s">
         <v>181</v>
       </c>
       <c r="G76" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="77">
@@ -2567,7 +2567,7 @@
         <v>181</v>
       </c>
       <c r="G78" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="79">
@@ -2607,13 +2607,13 @@
         <v>135</v>
       </c>
       <c r="E80" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F80" t="s">
         <v>181</v>
       </c>
       <c r="G80" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="81">
@@ -2659,7 +2659,7 @@
         <v>181</v>
       </c>
       <c r="G82" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="83">
@@ -2705,7 +2705,7 @@
         <v>181</v>
       </c>
       <c r="G84" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="85">
@@ -2751,7 +2751,7 @@
         <v>181</v>
       </c>
       <c r="G86" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="87">
@@ -2797,7 +2797,7 @@
         <v>181</v>
       </c>
       <c r="G88" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="89">
@@ -2843,7 +2843,7 @@
         <v>181</v>
       </c>
       <c r="G90" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="91">
@@ -2889,7 +2889,7 @@
         <v>181</v>
       </c>
       <c r="G92" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
     </row>
     <row r="93">
@@ -3073,7 +3073,7 @@
         <v>181</v>
       </c>
       <c r="G100" t="s">
-        <v>194</v>
+        <v>225</v>
       </c>
     </row>
     <row r="101">
@@ -3113,13 +3113,13 @@
         <v>135</v>
       </c>
       <c r="E102" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F102" t="s">
         <v>181</v>
       </c>
       <c r="G102" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="103">
@@ -3136,7 +3136,7 @@
         <v>0</v>
       </c>
       <c r="E103" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="F103" t="s">
         <v>0</v>
@@ -3159,13 +3159,13 @@
         <v>135</v>
       </c>
       <c r="E104" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F104" t="s">
         <v>181</v>
       </c>
       <c r="G104" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="105">
@@ -3211,7 +3211,7 @@
         <v>181</v>
       </c>
       <c r="G106" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="107">
@@ -3257,7 +3257,7 @@
         <v>181</v>
       </c>
       <c r="G108" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="109">
@@ -3303,7 +3303,7 @@
         <v>181</v>
       </c>
       <c r="G110" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="111">
@@ -3343,13 +3343,13 @@
         <v>135</v>
       </c>
       <c r="E112" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F112" t="s">
         <v>181</v>
       </c>
       <c r="G112" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
     </row>
     <row r="113">
@@ -3763,7 +3763,7 @@
         <v>181</v>
       </c>
       <c r="G130" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="131">

</xml_diff>